<commit_message>
24 Mayo 17 - Excel negociacion + Manejo errores cargue imagen usuario base 64
</commit_message>
<xml_diff>
--- a/Modelos/ConfiguracionBotonesNegociacion.xlsx
+++ b/Modelos/ConfiguracionBotonesNegociacion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9885" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9885" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Definicion" sheetId="1" r:id="rId1"/>
@@ -457,75 +457,75 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -799,7 +799,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -809,8 +809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28:C28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,11 +820,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
     </row>
     <row r="2" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -948,162 +948,162 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="30"/>
-      <c r="C14" s="30"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
         <v>-1</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="32"/>
+      <c r="C15" s="22"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
         <v>0</v>
       </c>
-      <c r="B16" s="32" t="s">
+      <c r="B16" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="32"/>
+      <c r="C16" s="22"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
         <v>1</v>
       </c>
-      <c r="B17" s="33" t="s">
+      <c r="B17" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="33"/>
+      <c r="C17" s="18"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="13">
         <v>3</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="34"/>
+      <c r="C18" s="21"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="13">
         <v>4</v>
       </c>
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="34"/>
+      <c r="C19" s="21"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="13">
         <v>7</v>
       </c>
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="34"/>
+      <c r="C20" s="21"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="11">
         <v>10</v>
       </c>
-      <c r="B21" s="33" t="s">
+      <c r="B21" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="33"/>
+      <c r="C21" s="18"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="30"/>
-      <c r="C23" s="30"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="11">
         <v>-1</v>
       </c>
-      <c r="B24" s="32" t="s">
+      <c r="B24" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="32"/>
+      <c r="C24" s="22"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
         <v>0</v>
       </c>
-      <c r="B25" s="32" t="s">
+      <c r="B25" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="32"/>
+      <c r="C25" s="22"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="11">
         <v>1</v>
       </c>
-      <c r="B26" s="33" t="s">
+      <c r="B26" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="33"/>
+      <c r="C26" s="18"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
         <v>2</v>
       </c>
-      <c r="B27" s="35" t="s">
+      <c r="B27" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="36"/>
+      <c r="C27" s="20"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="9">
         <v>5</v>
       </c>
-      <c r="B28" s="35" t="s">
+      <c r="B28" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="36"/>
+      <c r="C28" s="20"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="9">
         <v>6</v>
       </c>
-      <c r="B29" s="35" t="s">
+      <c r="B29" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C29" s="36"/>
+      <c r="C29" s="20"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="11">
         <v>10</v>
       </c>
-      <c r="B30" s="33" t="s">
+      <c r="B30" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="33"/>
+      <c r="C30" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -1116,8 +1116,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18:C24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1136,60 +1136,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="39" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="27"/>
+      <c r="A3" s="39"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="39"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="19">
+      <c r="A4" s="26">
         <v>-1</v>
       </c>
-      <c r="B4" s="37" t="str">
+      <c r="B4" s="31" t="str">
         <f>+VLOOKUP(A4,Definicion!$A$3:$C$12,3,0)</f>
         <v>Mensaje de texto normal (El que existe actualente para enviar un mensaje en el chat)</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="26" t="s">
         <v>34</v>
       </c>
       <c r="E4" s="4">
@@ -1204,10 +1204,10 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="38"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
       <c r="E5" s="2">
         <v>0</v>
       </c>
@@ -1220,10 +1220,10 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="38"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
+      <c r="A6" s="27"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
       <c r="E6" s="4">
         <v>1</v>
       </c>
@@ -1236,9 +1236,9 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
+      <c r="A7" s="27"/>
       <c r="B7" s="5"/>
-      <c r="C7" s="20"/>
+      <c r="C7" s="27"/>
       <c r="D7" s="5"/>
       <c r="E7" s="2">
         <v>3</v>
@@ -1252,9 +1252,9 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
+      <c r="A8" s="27"/>
       <c r="B8" s="5"/>
-      <c r="C8" s="20"/>
+      <c r="C8" s="27"/>
       <c r="D8" s="5"/>
       <c r="E8" s="4">
         <v>4</v>
@@ -1268,9 +1268,9 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
+      <c r="A9" s="27"/>
       <c r="B9" s="5"/>
-      <c r="C9" s="20"/>
+      <c r="C9" s="27"/>
       <c r="D9" s="5"/>
       <c r="E9" s="2">
         <v>7</v>
@@ -1284,9 +1284,9 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
+      <c r="A10" s="28"/>
       <c r="B10" s="6"/>
-      <c r="C10" s="21"/>
+      <c r="C10" s="28"/>
       <c r="D10" s="6"/>
       <c r="E10" s="4">
         <v>10</v>
@@ -1300,17 +1300,17 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22">
+      <c r="A11" s="24">
         <v>0</v>
       </c>
-      <c r="B11" s="39" t="str">
+      <c r="B11" s="33" t="str">
         <f>+VLOOKUP(A11,Definicion!$A$3:$C$12,3,0)</f>
         <v>Cancelar el trato actual</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="24" t="s">
         <v>29</v>
       </c>
       <c r="E11" s="2">
@@ -1325,10 +1325,10 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
-      <c r="B12" s="40"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
+      <c r="A12" s="25"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
       <c r="E12" s="4">
         <v>0</v>
       </c>
@@ -1341,9 +1341,9 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="7"/>
-      <c r="C13" s="23"/>
+      <c r="C13" s="25"/>
       <c r="D13" s="7"/>
       <c r="E13" s="2">
         <v>1</v>
@@ -1357,9 +1357,9 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="23"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="7"/>
-      <c r="C14" s="23"/>
+      <c r="C14" s="25"/>
       <c r="D14" s="7"/>
       <c r="E14" s="4">
         <v>3</v>
@@ -1373,9 +1373,9 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="23"/>
+      <c r="A15" s="25"/>
       <c r="B15" s="7"/>
-      <c r="C15" s="23"/>
+      <c r="C15" s="25"/>
       <c r="D15" s="7"/>
       <c r="E15" s="2">
         <v>4</v>
@@ -1389,9 +1389,9 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
+      <c r="A16" s="25"/>
       <c r="B16" s="7"/>
-      <c r="C16" s="23"/>
+      <c r="C16" s="25"/>
       <c r="D16" s="7"/>
       <c r="E16" s="4">
         <v>7</v>
@@ -1405,9 +1405,9 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="24"/>
+      <c r="A17" s="36"/>
       <c r="B17" s="8"/>
-      <c r="C17" s="24"/>
+      <c r="C17" s="36"/>
       <c r="D17" s="8"/>
       <c r="E17" s="2">
         <v>10</v>
@@ -1421,17 +1421,17 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="19">
+      <c r="A18" s="26">
         <v>1</v>
       </c>
-      <c r="B18" s="37" t="str">
+      <c r="B18" s="31" t="str">
         <f>+VLOOKUP(A18,Definicion!$A$3:$C$12,3,0)</f>
         <v>Aceptar el trato</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="26" t="s">
         <v>34</v>
       </c>
       <c r="E18" s="4">
@@ -1446,10 +1446,10 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="20"/>
-      <c r="B19" s="38"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
       <c r="E19" s="2">
         <v>0</v>
       </c>
@@ -1462,10 +1462,10 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="20"/>
-      <c r="B20" s="38"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
+      <c r="A20" s="27"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
       <c r="E20" s="4">
         <v>1</v>
       </c>
@@ -1478,9 +1478,9 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="20"/>
+      <c r="A21" s="27"/>
       <c r="B21" s="5"/>
-      <c r="C21" s="20"/>
+      <c r="C21" s="27"/>
       <c r="D21" s="5"/>
       <c r="E21" s="2">
         <v>3</v>
@@ -1494,9 +1494,9 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="20"/>
+      <c r="A22" s="27"/>
       <c r="B22" s="5"/>
-      <c r="C22" s="20"/>
+      <c r="C22" s="27"/>
       <c r="D22" s="5"/>
       <c r="E22" s="4">
         <v>4</v>
@@ -1510,9 +1510,9 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="20"/>
+      <c r="A23" s="27"/>
       <c r="B23" s="5"/>
-      <c r="C23" s="20"/>
+      <c r="C23" s="27"/>
       <c r="D23" s="5"/>
       <c r="E23" s="2">
         <v>7</v>
@@ -1526,9 +1526,9 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="21"/>
+      <c r="A24" s="28"/>
       <c r="B24" s="6"/>
-      <c r="C24" s="21"/>
+      <c r="C24" s="28"/>
       <c r="D24" s="6"/>
       <c r="E24" s="4">
         <v>10</v>
@@ -1542,17 +1542,17 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="22">
+      <c r="A25" s="24">
         <v>2</v>
       </c>
-      <c r="B25" s="39" t="str">
+      <c r="B25" s="33" t="str">
         <f>+VLOOKUP(A25,Definicion!$A$3:$C$12,3,0)</f>
         <v>Ofertar un valor por un ejemplar</v>
       </c>
-      <c r="C25" s="22" t="s">
+      <c r="C25" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="D25" s="22" t="s">
+      <c r="D25" s="24" t="s">
         <v>37</v>
       </c>
       <c r="E25" s="2">
@@ -1567,10 +1567,10 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="23"/>
-      <c r="B26" s="40"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
+      <c r="A26" s="25"/>
+      <c r="B26" s="34"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
       <c r="E26" s="4">
         <v>0</v>
       </c>
@@ -1583,10 +1583,10 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="23"/>
-      <c r="B27" s="40"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
+      <c r="A27" s="25"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
       <c r="E27" s="2">
         <v>1</v>
       </c>
@@ -1599,10 +1599,10 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
-      <c r="B28" s="40"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
+      <c r="A28" s="25"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
       <c r="E28" s="4">
         <v>3</v>
       </c>
@@ -1615,9 +1615,9 @@
       </c>
     </row>
     <row r="29" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="23"/>
+      <c r="A29" s="25"/>
       <c r="B29" s="7"/>
-      <c r="C29" s="23"/>
+      <c r="C29" s="25"/>
       <c r="D29" s="7"/>
       <c r="E29" s="2">
         <v>4</v>
@@ -1631,9 +1631,9 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="23"/>
+      <c r="A30" s="25"/>
       <c r="B30" s="7"/>
-      <c r="C30" s="23"/>
+      <c r="C30" s="25"/>
       <c r="D30" s="7"/>
       <c r="E30" s="4">
         <v>7</v>
@@ -1647,9 +1647,9 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="24"/>
+      <c r="A31" s="36"/>
       <c r="B31" s="8"/>
-      <c r="C31" s="24"/>
+      <c r="C31" s="36"/>
       <c r="D31" s="8"/>
       <c r="E31" s="2">
         <v>10</v>
@@ -1663,17 +1663,17 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="19">
+      <c r="A32" s="26">
         <v>5</v>
       </c>
-      <c r="B32" s="37" t="str">
+      <c r="B32" s="31" t="str">
         <f>+VLOOKUP(A32,Definicion!$A$3:$C$12,3,0)</f>
         <v>Recibir el ejemplar (Se informa a la plataforma que físicamente se recibió)</v>
       </c>
-      <c r="C32" s="19" t="s">
+      <c r="C32" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="D32" s="19" t="s">
+      <c r="D32" s="26" t="s">
         <v>38</v>
       </c>
       <c r="E32" s="4">
@@ -1688,10 +1688,10 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="20"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
+      <c r="A33" s="27"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
       <c r="E33" s="2">
         <v>0</v>
       </c>
@@ -1704,10 +1704,10 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="20"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
+      <c r="A34" s="27"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
       <c r="E34" s="4">
         <v>1</v>
       </c>
@@ -1720,10 +1720,10 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="20"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
+      <c r="A35" s="27"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
       <c r="E35" s="2">
         <v>3</v>
       </c>
@@ -1736,10 +1736,10 @@
       </c>
     </row>
     <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="20"/>
-      <c r="B36" s="38"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
+      <c r="A36" s="27"/>
+      <c r="B36" s="32"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="27"/>
       <c r="E36" s="4">
         <v>4</v>
       </c>
@@ -1752,9 +1752,9 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="20"/>
+      <c r="A37" s="27"/>
       <c r="B37" s="5"/>
-      <c r="C37" s="20"/>
+      <c r="C37" s="27"/>
       <c r="D37" s="5"/>
       <c r="E37" s="2">
         <v>7</v>
@@ -1768,9 +1768,9 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="21"/>
+      <c r="A38" s="28"/>
       <c r="B38" s="6"/>
-      <c r="C38" s="21"/>
+      <c r="C38" s="28"/>
       <c r="D38" s="6"/>
       <c r="E38" s="4">
         <v>10</v>
@@ -1784,17 +1784,17 @@
       </c>
     </row>
     <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="22">
+      <c r="A39" s="24">
         <v>6</v>
       </c>
-      <c r="B39" s="39" t="str">
+      <c r="B39" s="33" t="str">
         <f>+VLOOKUP(A39,Definicion!$A$3:$C$12,3,0)</f>
         <v>Calificación (El solicitante califica)</v>
       </c>
-      <c r="C39" s="22" t="s">
+      <c r="C39" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="D39" s="22" t="s">
+      <c r="D39" s="24" t="s">
         <v>36</v>
       </c>
       <c r="E39" s="2">
@@ -1809,10 +1809,10 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="23"/>
-      <c r="B40" s="23"/>
-      <c r="C40" s="23"/>
-      <c r="D40" s="23"/>
+      <c r="A40" s="25"/>
+      <c r="B40" s="25"/>
+      <c r="C40" s="25"/>
+      <c r="D40" s="25"/>
       <c r="E40" s="4">
         <v>0</v>
       </c>
@@ -1825,10 +1825,10 @@
       </c>
     </row>
     <row r="41" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="23"/>
-      <c r="B41" s="23"/>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23"/>
+      <c r="A41" s="25"/>
+      <c r="B41" s="25"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="25"/>
       <c r="E41" s="2">
         <v>1</v>
       </c>
@@ -1841,10 +1841,10 @@
       </c>
     </row>
     <row r="42" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="23"/>
-      <c r="B42" s="23"/>
-      <c r="C42" s="23"/>
-      <c r="D42" s="23"/>
+      <c r="A42" s="25"/>
+      <c r="B42" s="25"/>
+      <c r="C42" s="25"/>
+      <c r="D42" s="25"/>
       <c r="E42" s="4">
         <v>3</v>
       </c>
@@ -1857,10 +1857,10 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23"/>
-      <c r="C43" s="23"/>
-      <c r="D43" s="23"/>
+      <c r="A43" s="25"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="25"/>
+      <c r="D43" s="25"/>
       <c r="E43" s="2">
         <v>4</v>
       </c>
@@ -1873,10 +1873,10 @@
       </c>
     </row>
     <row r="44" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="23"/>
-      <c r="B44" s="40"/>
-      <c r="C44" s="23"/>
-      <c r="D44" s="23"/>
+      <c r="A44" s="25"/>
+      <c r="B44" s="34"/>
+      <c r="C44" s="25"/>
+      <c r="D44" s="25"/>
       <c r="E44" s="4">
         <v>7</v>
       </c>
@@ -1889,9 +1889,9 @@
       </c>
     </row>
     <row r="45" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="24"/>
+      <c r="A45" s="36"/>
       <c r="B45" s="8"/>
-      <c r="C45" s="24"/>
+      <c r="C45" s="36"/>
       <c r="D45" s="8"/>
       <c r="E45" s="2">
         <v>10</v>
@@ -1905,17 +1905,17 @@
       </c>
     </row>
     <row r="46" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="19">
+      <c r="A46" s="26">
         <v>10</v>
       </c>
-      <c r="B46" s="37" t="str">
+      <c r="B46" s="31" t="str">
         <f>+VLOOKUP(A46,Definicion!$A$3:$C$12,3,0)</f>
         <v>TRATO FINALIZADO</v>
       </c>
-      <c r="C46" s="19" t="s">
+      <c r="C46" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="D46" s="19" t="s">
+      <c r="D46" s="26" t="s">
         <v>31</v>
       </c>
       <c r="E46" s="4">
@@ -1930,10 +1930,10 @@
       </c>
     </row>
     <row r="47" spans="1:7" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="20"/>
-      <c r="B47" s="20"/>
-      <c r="C47" s="20"/>
-      <c r="D47" s="20"/>
+      <c r="A47" s="27"/>
+      <c r="B47" s="27"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="27"/>
       <c r="E47" s="2">
         <v>0</v>
       </c>
@@ -1946,10 +1946,10 @@
       </c>
     </row>
     <row r="48" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="20"/>
-      <c r="B48" s="20"/>
-      <c r="C48" s="20"/>
-      <c r="D48" s="20"/>
+      <c r="A48" s="27"/>
+      <c r="B48" s="27"/>
+      <c r="C48" s="27"/>
+      <c r="D48" s="27"/>
       <c r="E48" s="4">
         <v>1</v>
       </c>
@@ -1962,10 +1962,10 @@
       </c>
     </row>
     <row r="49" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="20"/>
-      <c r="B49" s="20"/>
-      <c r="C49" s="20"/>
-      <c r="D49" s="20"/>
+      <c r="A49" s="27"/>
+      <c r="B49" s="27"/>
+      <c r="C49" s="27"/>
+      <c r="D49" s="27"/>
       <c r="E49" s="2">
         <v>3</v>
       </c>
@@ -1978,10 +1978,10 @@
       </c>
     </row>
     <row r="50" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="20"/>
-      <c r="B50" s="20"/>
-      <c r="C50" s="20"/>
-      <c r="D50" s="20"/>
+      <c r="A50" s="27"/>
+      <c r="B50" s="27"/>
+      <c r="C50" s="27"/>
+      <c r="D50" s="27"/>
       <c r="E50" s="4">
         <v>4</v>
       </c>
@@ -1994,10 +1994,10 @@
       </c>
     </row>
     <row r="51" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="20"/>
-      <c r="B51" s="20"/>
-      <c r="C51" s="20"/>
-      <c r="D51" s="20"/>
+      <c r="A51" s="27"/>
+      <c r="B51" s="27"/>
+      <c r="C51" s="27"/>
+      <c r="D51" s="27"/>
       <c r="E51" s="2">
         <v>7</v>
       </c>
@@ -2010,10 +2010,10 @@
       </c>
     </row>
     <row r="52" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="21"/>
-      <c r="B52" s="41"/>
-      <c r="C52" s="21"/>
-      <c r="D52" s="21"/>
+      <c r="A52" s="28"/>
+      <c r="B52" s="35"/>
+      <c r="C52" s="28"/>
+      <c r="D52" s="28"/>
       <c r="E52" s="4">
         <v>10</v>
       </c>
@@ -2028,19 +2028,26 @@
   </sheetData>
   <autoFilter ref="A2:G52">
     <filterColumn colId="6">
-      <filters blank="1">
+      <filters>
         <filter val="S"/>
       </filters>
     </filterColumn>
   </autoFilter>
   <mergeCells count="36">
-    <mergeCell ref="D39:D44"/>
-    <mergeCell ref="D46:D52"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="D25:D28"/>
-    <mergeCell ref="D32:D36"/>
+    <mergeCell ref="A46:A52"/>
+    <mergeCell ref="A4:A10"/>
+    <mergeCell ref="A11:A17"/>
+    <mergeCell ref="A18:A24"/>
+    <mergeCell ref="A25:A31"/>
+    <mergeCell ref="A32:A38"/>
+    <mergeCell ref="A39:A45"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
     <mergeCell ref="C46:C52"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="B4:B6"/>
@@ -2055,23 +2062,17 @@
     <mergeCell ref="C25:C31"/>
     <mergeCell ref="C32:C38"/>
     <mergeCell ref="C39:C45"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="A46:A52"/>
-    <mergeCell ref="A4:A10"/>
-    <mergeCell ref="A11:A17"/>
-    <mergeCell ref="A18:A24"/>
-    <mergeCell ref="A25:A31"/>
-    <mergeCell ref="A32:A38"/>
-    <mergeCell ref="A39:A45"/>
     <mergeCell ref="C4:C10"/>
+    <mergeCell ref="D39:D44"/>
+    <mergeCell ref="D46:D52"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="D25:D28"/>
+    <mergeCell ref="D32:D36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2080,7 +2081,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
@@ -2096,60 +2097,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
     </row>
     <row r="2" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="39" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="27"/>
+      <c r="A3" s="39"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="39"/>
     </row>
     <row r="4" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="19">
+      <c r="A4" s="26">
         <v>-1</v>
       </c>
-      <c r="B4" s="37" t="str">
+      <c r="B4" s="31" t="str">
         <f>+VLOOKUP(A4,Definicion!$A$3:$C$12,3,0)</f>
         <v>Mensaje de texto normal (El que existe actualente para enviar un mensaje en el chat)</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="26" t="s">
         <v>28</v>
       </c>
       <c r="E4" s="4">
@@ -2164,10 +2165,10 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="38"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
       <c r="E5" s="2">
         <v>0</v>
       </c>
@@ -2180,10 +2181,10 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="38"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
+      <c r="A6" s="27"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
       <c r="E6" s="4">
         <v>1</v>
       </c>
@@ -2196,10 +2197,10 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
-      <c r="B7" s="38"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
+      <c r="A7" s="27"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
       <c r="E7" s="2">
         <v>2</v>
       </c>
@@ -2212,9 +2213,9 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
+      <c r="A8" s="27"/>
       <c r="B8" s="5"/>
-      <c r="C8" s="20"/>
+      <c r="C8" s="27"/>
       <c r="D8" s="5"/>
       <c r="E8" s="4">
         <v>5</v>
@@ -2228,9 +2229,9 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
+      <c r="A9" s="27"/>
       <c r="B9" s="5"/>
-      <c r="C9" s="20"/>
+      <c r="C9" s="27"/>
       <c r="D9" s="5"/>
       <c r="E9" s="2">
         <v>6</v>
@@ -2244,9 +2245,9 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
+      <c r="A10" s="28"/>
       <c r="B10" s="6"/>
-      <c r="C10" s="21"/>
+      <c r="C10" s="28"/>
       <c r="D10" s="6"/>
       <c r="E10" s="4">
         <v>10</v>
@@ -2260,17 +2261,17 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22">
+      <c r="A11" s="24">
         <v>0</v>
       </c>
-      <c r="B11" s="39" t="str">
+      <c r="B11" s="33" t="str">
         <f>+VLOOKUP(A11,Definicion!$A$3:$C$12,3,0)</f>
         <v>Cancelar el trato actual</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="24" t="s">
         <v>29</v>
       </c>
       <c r="E11" s="2">
@@ -2285,10 +2286,10 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
-      <c r="B12" s="40"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
+      <c r="A12" s="25"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
       <c r="E12" s="4">
         <v>0</v>
       </c>
@@ -2301,9 +2302,9 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="7"/>
-      <c r="C13" s="23"/>
+      <c r="C13" s="25"/>
       <c r="D13" s="7"/>
       <c r="E13" s="2">
         <v>1</v>
@@ -2317,9 +2318,9 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="23"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="7"/>
-      <c r="C14" s="23"/>
+      <c r="C14" s="25"/>
       <c r="D14" s="7"/>
       <c r="E14" s="4">
         <v>2</v>
@@ -2333,9 +2334,9 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="23"/>
+      <c r="A15" s="25"/>
       <c r="B15" s="7"/>
-      <c r="C15" s="23"/>
+      <c r="C15" s="25"/>
       <c r="D15" s="7"/>
       <c r="E15" s="2">
         <v>5</v>
@@ -2349,9 +2350,9 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
+      <c r="A16" s="25"/>
       <c r="B16" s="7"/>
-      <c r="C16" s="23"/>
+      <c r="C16" s="25"/>
       <c r="D16" s="7"/>
       <c r="E16" s="4">
         <v>6</v>
@@ -2365,9 +2366,9 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="24"/>
+      <c r="A17" s="36"/>
       <c r="B17" s="8"/>
-      <c r="C17" s="24"/>
+      <c r="C17" s="36"/>
       <c r="D17" s="8"/>
       <c r="E17" s="2">
         <v>10</v>
@@ -2381,17 +2382,17 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="19">
+      <c r="A18" s="26">
         <v>1</v>
       </c>
-      <c r="B18" s="37" t="str">
+      <c r="B18" s="31" t="str">
         <f>+VLOOKUP(A18,Definicion!$A$3:$C$12,3,0)</f>
         <v>Aceptar el trato</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="26" t="s">
         <v>34</v>
       </c>
       <c r="E18" s="4">
@@ -2406,10 +2407,10 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="20"/>
-      <c r="B19" s="38"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
       <c r="E19" s="2">
         <v>0</v>
       </c>
@@ -2422,10 +2423,10 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="20"/>
-      <c r="B20" s="38"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
+      <c r="A20" s="27"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
       <c r="E20" s="4">
         <v>1</v>
       </c>
@@ -2438,10 +2439,10 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="20"/>
+      <c r="A21" s="27"/>
       <c r="B21" s="5"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
       <c r="E21" s="2">
         <v>2</v>
       </c>
@@ -2454,9 +2455,9 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="20"/>
+      <c r="A22" s="27"/>
       <c r="B22" s="5"/>
-      <c r="C22" s="20"/>
+      <c r="C22" s="27"/>
       <c r="D22" s="5"/>
       <c r="E22" s="4">
         <v>5</v>
@@ -2470,9 +2471,9 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="20"/>
+      <c r="A23" s="27"/>
       <c r="B23" s="5"/>
-      <c r="C23" s="20"/>
+      <c r="C23" s="27"/>
       <c r="D23" s="5"/>
       <c r="E23" s="2">
         <v>6</v>
@@ -2486,9 +2487,9 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="21"/>
+      <c r="A24" s="28"/>
       <c r="B24" s="6"/>
-      <c r="C24" s="21"/>
+      <c r="C24" s="28"/>
       <c r="D24" s="6"/>
       <c r="E24" s="4">
         <v>10</v>
@@ -2502,17 +2503,17 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="22">
+      <c r="A25" s="24">
         <v>3</v>
       </c>
-      <c r="B25" s="39" t="str">
+      <c r="B25" s="33" t="str">
         <f>+VLOOKUP(A25,Definicion!$A$3:$C$12,3,0)</f>
         <v>Contraofertar una oferta realizada por el Solicitante</v>
       </c>
-      <c r="C25" s="22" t="s">
+      <c r="C25" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="22" t="s">
+      <c r="D25" s="24" t="s">
         <v>28</v>
       </c>
       <c r="E25" s="2">
@@ -2527,10 +2528,10 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="23"/>
-      <c r="B26" s="40"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
+      <c r="A26" s="25"/>
+      <c r="B26" s="34"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
       <c r="E26" s="4">
         <v>0</v>
       </c>
@@ -2543,10 +2544,10 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="23"/>
-      <c r="B27" s="40"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
+      <c r="A27" s="25"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
       <c r="E27" s="2">
         <v>1</v>
       </c>
@@ -2559,10 +2560,10 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
-      <c r="B28" s="40"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
+      <c r="A28" s="25"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
       <c r="E28" s="4">
         <v>2</v>
       </c>
@@ -2575,9 +2576,9 @@
       </c>
     </row>
     <row r="29" spans="1:7" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="23"/>
+      <c r="A29" s="25"/>
       <c r="B29" s="7"/>
-      <c r="C29" s="23"/>
+      <c r="C29" s="25"/>
       <c r="D29" s="7"/>
       <c r="E29" s="2">
         <v>5</v>
@@ -2591,9 +2592,9 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="23"/>
+      <c r="A30" s="25"/>
       <c r="B30" s="7"/>
-      <c r="C30" s="23"/>
+      <c r="C30" s="25"/>
       <c r="D30" s="7"/>
       <c r="E30" s="4">
         <v>6</v>
@@ -2607,9 +2608,9 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="24"/>
+      <c r="A31" s="36"/>
       <c r="B31" s="8"/>
-      <c r="C31" s="24"/>
+      <c r="C31" s="36"/>
       <c r="D31" s="8"/>
       <c r="E31" s="2">
         <v>10</v>
@@ -2623,17 +2624,17 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="19">
-        <v>4</v>
-      </c>
-      <c r="B32" s="37" t="str">
+      <c r="A32" s="26">
+        <v>4</v>
+      </c>
+      <c r="B32" s="31" t="str">
         <f>+VLOOKUP(A32,Definicion!$A$3:$C$12,3,0)</f>
         <v>Entregar el ejemplar (Se informa a la plataforma que físicamente se entrego)</v>
       </c>
-      <c r="C32" s="19" t="s">
+      <c r="C32" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="D32" s="19" t="s">
+      <c r="D32" s="26" t="s">
         <v>39</v>
       </c>
       <c r="E32" s="4">
@@ -2648,10 +2649,10 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="20"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
+      <c r="A33" s="27"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
       <c r="E33" s="2">
         <v>0</v>
       </c>
@@ -2664,10 +2665,10 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="20"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
+      <c r="A34" s="27"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
       <c r="E34" s="4">
         <v>1</v>
       </c>
@@ -2680,10 +2681,10 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="20"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
+      <c r="A35" s="27"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
       <c r="E35" s="2">
         <v>2</v>
       </c>
@@ -2696,10 +2697,10 @@
       </c>
     </row>
     <row r="36" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="20"/>
-      <c r="B36" s="38"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
+      <c r="A36" s="27"/>
+      <c r="B36" s="32"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="27"/>
       <c r="E36" s="4">
         <v>5</v>
       </c>
@@ -2712,9 +2713,9 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="20"/>
+      <c r="A37" s="27"/>
       <c r="B37" s="5"/>
-      <c r="C37" s="20"/>
+      <c r="C37" s="27"/>
       <c r="D37" s="5"/>
       <c r="E37" s="2">
         <v>6</v>
@@ -2728,9 +2729,9 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="21"/>
+      <c r="A38" s="28"/>
       <c r="B38" s="6"/>
-      <c r="C38" s="21"/>
+      <c r="C38" s="28"/>
       <c r="D38" s="6"/>
       <c r="E38" s="4">
         <v>10</v>
@@ -2744,17 +2745,17 @@
       </c>
     </row>
     <row r="39" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="22">
+      <c r="A39" s="24">
         <v>7</v>
       </c>
-      <c r="B39" s="39" t="str">
+      <c r="B39" s="33" t="str">
         <f>+VLOOKUP(A39,Definicion!$A$3:$C$12,3,0)</f>
         <v>Calificación (El dueño califica)</v>
       </c>
-      <c r="C39" s="22" t="s">
+      <c r="C39" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="D39" s="22" t="s">
+      <c r="D39" s="24" t="s">
         <v>38</v>
       </c>
       <c r="E39" s="2">
@@ -2769,10 +2770,10 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="23"/>
-      <c r="B40" s="23"/>
-      <c r="C40" s="23"/>
-      <c r="D40" s="23"/>
+      <c r="A40" s="25"/>
+      <c r="B40" s="25"/>
+      <c r="C40" s="25"/>
+      <c r="D40" s="25"/>
       <c r="E40" s="4">
         <v>0</v>
       </c>
@@ -2785,10 +2786,10 @@
       </c>
     </row>
     <row r="41" spans="1:7" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="23"/>
-      <c r="B41" s="23"/>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23"/>
+      <c r="A41" s="25"/>
+      <c r="B41" s="25"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="25"/>
       <c r="E41" s="2">
         <v>1</v>
       </c>
@@ -2801,10 +2802,10 @@
       </c>
     </row>
     <row r="42" spans="1:7" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="23"/>
-      <c r="B42" s="23"/>
-      <c r="C42" s="23"/>
-      <c r="D42" s="23"/>
+      <c r="A42" s="25"/>
+      <c r="B42" s="25"/>
+      <c r="C42" s="25"/>
+      <c r="D42" s="25"/>
       <c r="E42" s="4">
         <v>2</v>
       </c>
@@ -2817,10 +2818,10 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23"/>
-      <c r="C43" s="23"/>
-      <c r="D43" s="23"/>
+      <c r="A43" s="25"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="25"/>
+      <c r="D43" s="25"/>
       <c r="E43" s="2">
         <v>5</v>
       </c>
@@ -2833,10 +2834,10 @@
       </c>
     </row>
     <row r="44" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="23"/>
-      <c r="B44" s="40"/>
-      <c r="C44" s="23"/>
-      <c r="D44" s="23"/>
+      <c r="A44" s="25"/>
+      <c r="B44" s="34"/>
+      <c r="C44" s="25"/>
+      <c r="D44" s="25"/>
       <c r="E44" s="4">
         <v>6</v>
       </c>
@@ -2849,9 +2850,9 @@
       </c>
     </row>
     <row r="45" spans="1:7" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="24"/>
+      <c r="A45" s="36"/>
       <c r="B45" s="8"/>
-      <c r="C45" s="24"/>
+      <c r="C45" s="36"/>
       <c r="D45" s="8"/>
       <c r="E45" s="2">
         <v>10</v>
@@ -2865,17 +2866,17 @@
       </c>
     </row>
     <row r="46" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="19">
+      <c r="A46" s="26">
         <v>10</v>
       </c>
-      <c r="B46" s="37" t="str">
+      <c r="B46" s="31" t="str">
         <f>+VLOOKUP(A46,Definicion!$A$3:$C$12,3,0)</f>
         <v>TRATO FINALIZADO</v>
       </c>
-      <c r="C46" s="19" t="s">
+      <c r="C46" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="D46" s="19" t="s">
+      <c r="D46" s="26" t="s">
         <v>31</v>
       </c>
       <c r="E46" s="4">
@@ -2890,10 +2891,10 @@
       </c>
     </row>
     <row r="47" spans="1:7" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="20"/>
-      <c r="B47" s="20"/>
-      <c r="C47" s="20"/>
-      <c r="D47" s="20"/>
+      <c r="A47" s="27"/>
+      <c r="B47" s="27"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="27"/>
       <c r="E47" s="2">
         <v>0</v>
       </c>
@@ -2906,10 +2907,10 @@
       </c>
     </row>
     <row r="48" spans="1:7" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="20"/>
-      <c r="B48" s="20"/>
-      <c r="C48" s="20"/>
-      <c r="D48" s="20"/>
+      <c r="A48" s="27"/>
+      <c r="B48" s="27"/>
+      <c r="C48" s="27"/>
+      <c r="D48" s="27"/>
       <c r="E48" s="4">
         <v>1</v>
       </c>
@@ -2922,10 +2923,10 @@
       </c>
     </row>
     <row r="49" spans="1:7" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="20"/>
-      <c r="B49" s="20"/>
-      <c r="C49" s="20"/>
-      <c r="D49" s="20"/>
+      <c r="A49" s="27"/>
+      <c r="B49" s="27"/>
+      <c r="C49" s="27"/>
+      <c r="D49" s="27"/>
       <c r="E49" s="2">
         <v>2</v>
       </c>
@@ -2938,10 +2939,10 @@
       </c>
     </row>
     <row r="50" spans="1:7" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="20"/>
-      <c r="B50" s="20"/>
-      <c r="C50" s="20"/>
-      <c r="D50" s="20"/>
+      <c r="A50" s="27"/>
+      <c r="B50" s="27"/>
+      <c r="C50" s="27"/>
+      <c r="D50" s="27"/>
       <c r="E50" s="4">
         <v>5</v>
       </c>
@@ -2954,10 +2955,10 @@
       </c>
     </row>
     <row r="51" spans="1:7" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="20"/>
-      <c r="B51" s="20"/>
-      <c r="C51" s="20"/>
-      <c r="D51" s="20"/>
+      <c r="A51" s="27"/>
+      <c r="B51" s="27"/>
+      <c r="C51" s="27"/>
+      <c r="D51" s="27"/>
       <c r="E51" s="2">
         <v>6</v>
       </c>
@@ -2970,10 +2971,10 @@
       </c>
     </row>
     <row r="52" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="21"/>
-      <c r="B52" s="41"/>
-      <c r="C52" s="21"/>
-      <c r="D52" s="21"/>
+      <c r="A52" s="28"/>
+      <c r="B52" s="35"/>
+      <c r="C52" s="28"/>
+      <c r="D52" s="28"/>
       <c r="E52" s="4">
         <v>10</v>
       </c>
@@ -2988,18 +2989,27 @@
   </sheetData>
   <autoFilter ref="A2:G52">
     <filterColumn colId="6">
-      <filters blank="1">
+      <filters>
         <filter val="S"/>
       </filters>
     </filterColumn>
   </autoFilter>
   <mergeCells count="36">
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="D25:D28"/>
-    <mergeCell ref="D32:D36"/>
-    <mergeCell ref="D39:D44"/>
-    <mergeCell ref="D46:D52"/>
-    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="D4:D7"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="A32:A38"/>
+    <mergeCell ref="A39:A45"/>
+    <mergeCell ref="A46:A52"/>
+    <mergeCell ref="A4:A10"/>
+    <mergeCell ref="A11:A17"/>
+    <mergeCell ref="A18:A24"/>
+    <mergeCell ref="A25:A31"/>
     <mergeCell ref="C46:C52"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="B4:B7"/>
@@ -3015,21 +3025,12 @@
     <mergeCell ref="C25:C31"/>
     <mergeCell ref="C32:C38"/>
     <mergeCell ref="C39:C45"/>
-    <mergeCell ref="A32:A38"/>
-    <mergeCell ref="A39:A45"/>
-    <mergeCell ref="A46:A52"/>
-    <mergeCell ref="A4:A10"/>
-    <mergeCell ref="A11:A17"/>
-    <mergeCell ref="A18:A24"/>
-    <mergeCell ref="A25:A31"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="D4:D7"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="D25:D28"/>
+    <mergeCell ref="D32:D36"/>
+    <mergeCell ref="D39:D44"/>
+    <mergeCell ref="D46:D52"/>
+    <mergeCell ref="D18:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>